<commit_message>
Update mods data [2025-11-12 07:50:19]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -1,52 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ModCounts" sheetId="1" r:id="rId1"/>
+    <sheet name="ModCounts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,14 +41,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,37 +443,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Game</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ModCount</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Game</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ModCount</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>2025/11/11</v>
-      </c>
-      <c r="B2" t="str">
-        <v>逃离鸭科夫</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1035</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025/11/11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1035</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/12</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1057</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mods data [2025-11-12 13:53:02]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -1,56 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ModCounts" sheetId="1" r:id="rId1"/>
+    <sheet name="ModCounts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -68,14 +41,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,37 +443,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Game</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ModCount</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Game</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ModCount</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>2025/11/11</v>
-      </c>
-      <c r="B2" t="str">
-        <v>逃离鸭科夫</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1035</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025/11/11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1035</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/12</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1063</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mods data [2025-11-12 15:10:51]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -1,52 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ModCounts" sheetId="1" r:id="rId1"/>
+    <sheet name="ModCounts" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -64,14 +41,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,37 +443,74 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="50" customWidth="1" min="1" max="1"/>
+    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Date</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Game</v>
-      </c>
-      <c r="C1" t="str">
-        <v>ModCount</v>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Game</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>ModCount</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>2025/11/11</v>
-      </c>
-      <c r="B2" t="str">
-        <v>逃离鸭科夫</v>
-      </c>
-      <c r="C2" t="str">
-        <v>1035</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025/11/11</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1035</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/12</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>1067</v>
       </c>
     </row>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
-  </ignoredErrors>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mods data [2025-11-13 15:11:24]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,6 +510,21 @@
         <v>1067</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/13</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>1081</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-14 15:09:55]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,6 +525,21 @@
         <v>1081</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/14</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>1089</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-15 15:07:59]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -540,6 +540,21 @@
         <v>1089</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/15</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>1119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-16 15:08:13]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,6 +555,21 @@
         <v>1119</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/16</t>
+        </is>
+      </c>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>1139</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-17 15:11:29]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,6 +570,21 @@
         <v>1139</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/17</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>1155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-18 15:10:56]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,21 @@
         <v>1155</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/18</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>1167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-20 15:10:21]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,6 +615,21 @@
         <v>1182</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/20</t>
+        </is>
+      </c>
+      <c r="B11" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>1196</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-21 15:09:52]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -630,6 +630,21 @@
         <v>1196</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/21</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>1211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-22 15:08:32]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -645,6 +645,21 @@
         <v>1211</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/22</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>1222</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-23 15:08:39]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,6 +660,21 @@
         <v>1222</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/23</t>
+        </is>
+      </c>
+      <c r="B14" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>1236</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-24 15:11:16]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,6 +675,21 @@
         <v>1236</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/24</t>
+        </is>
+      </c>
+      <c r="B15" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1242</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-25 15:10:55]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -690,6 +690,21 @@
         <v>1242</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/25</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1256</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-26 15:08:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -705,6 +705,21 @@
         <v>1256</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/26</t>
+        </is>
+      </c>
+      <c r="B17" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1263</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-27 15:10:15]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,6 +720,21 @@
         <v>1263</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/27</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>1270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-28 15:09:46]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,6 +735,21 @@
         <v>1270</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/28</t>
+        </is>
+      </c>
+      <c r="B19" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>1275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-29 15:08:54]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -750,6 +750,21 @@
         <v>1275</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/29</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>1276</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-11-30 15:09:01]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -765,6 +765,21 @@
         <v>1276</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>2025/11/30</t>
+        </is>
+      </c>
+      <c r="B21" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>1287</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-01 15:11:34]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,6 +780,21 @@
         <v>1287</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/01</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>1296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-02 15:11:55]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -795,6 +795,21 @@
         <v>1296</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/02</t>
+        </is>
+      </c>
+      <c r="B23" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>1310</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-03 15:12:04]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -810,6 +810,21 @@
         <v>1310</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/03</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>1322</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-04 15:12:45]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -825,6 +825,21 @@
         <v>1322</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/04</t>
+        </is>
+      </c>
+      <c r="B25" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>1327</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-05 15:10:54]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -840,6 +840,21 @@
         <v>1327</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/05</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>1332</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-06 15:08:39]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -855,6 +855,21 @@
         <v>1332</v>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/06</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>1336</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-07 15:08:30]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,6 +870,21 @@
         <v>1336</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/07</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>1343</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-08 15:11:36]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,6 +885,21 @@
         <v>1343</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/08</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>1349</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-09 15:12:17]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -900,6 +900,21 @@
         <v>1349</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/09</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>1351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-10 15:13:28]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -915,6 +915,21 @@
         <v>1351</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/10</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>1351</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-11 15:12:51]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -930,6 +930,21 @@
         <v>1351</v>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/11</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>1354</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-12 15:11:40]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -945,6 +945,21 @@
         <v>1354</v>
       </c>
     </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/12</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>1356</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-13 15:09:15]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -960,6 +960,21 @@
         <v>1356</v>
       </c>
     </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/13</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>1360</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-14 15:09:40]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -975,6 +975,21 @@
         <v>1360</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/14</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>1349</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-15 15:15:23]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -990,6 +990,21 @@
         <v>1349</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/15</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>1348</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-16 15:13:09]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1005,6 +1005,21 @@
         <v>1348</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/16</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>1343</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-17 15:12:04]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1020,6 +1020,21 @@
         <v>1343</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/17</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>1342</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-18 15:12:02]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1035,6 +1035,21 @@
         <v>1342</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/18</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>1345</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-19 15:11:08]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1050,6 +1050,21 @@
         <v>1345</v>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/19</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>1352</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-20 15:09:10]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1065,6 +1065,21 @@
         <v>1352</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/20</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>1357</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-21 15:09:08]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1080,6 +1080,21 @@
         <v>1357</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/21</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>1097</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-23 15:11:09]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1095,6 +1095,21 @@
         <v>1097</v>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/23</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>1095</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-24 15:11:08]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,6 +1110,21 @@
         <v>1095</v>
       </c>
     </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/24</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>1096</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-25 15:11:39]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1125,6 +1125,21 @@
         <v>1096</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/25</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>1100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-26 15:10:42]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1140,6 +1140,21 @@
         <v>1100</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/26</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>1102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-27 15:09:07]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1155,6 +1155,21 @@
         <v>1102</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/27</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>1104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-28 15:09:22]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1170,6 +1170,21 @@
         <v>1104</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/28</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>1112</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-29 15:11:27]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1185,6 +1185,21 @@
         <v>1112</v>
       </c>
     </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/29</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>1111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-30 15:11:10]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1200,6 +1200,21 @@
         <v>1111</v>
       </c>
     </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/30</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>1106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2025-12-31 15:11:06]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1215,6 +1215,21 @@
         <v>1106</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>2025/12/31</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>1121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-01 15:10:40]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1230,6 +1230,21 @@
         <v>1121</v>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/01</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>1123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-02 15:10:56]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1245,6 +1245,21 @@
         <v>1123</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/02</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>1127</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-03 15:09:14]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1260,6 +1260,21 @@
         <v>1127</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/03</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>1130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-04 15:09:16]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1275,6 +1275,21 @@
         <v>1130</v>
       </c>
     </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/04</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>1137</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-05 15:13:11]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1290,6 +1290,21 @@
         <v>1137</v>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/05</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>1135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-06 15:11:46]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1305,6 +1305,21 @@
         <v>1135</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/06</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>1138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-07 15:13:10]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1320,6 +1320,21 @@
         <v>1138</v>
       </c>
     </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/07</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>1140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-08 15:14:25]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1335,6 +1335,21 @@
         <v>1140</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/08</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>1140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-09 15:11:43]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C59"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1350,6 +1350,21 @@
         <v>1140</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/09</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>1140</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-10 15:09:14]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1365,6 +1365,21 @@
         <v>1140</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/10</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>1141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-11 15:09:21]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1380,6 +1380,21 @@
         <v>1141</v>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/11</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>1143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-12 15:14:48]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1395,6 +1395,21 @@
         <v>1143</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/12</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>1143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-13 15:13:42]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1410,6 +1410,21 @@
         <v>1143</v>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/13</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>1144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-14 15:14:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1425,6 +1425,21 @@
         <v>1144</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/14</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>1144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-15 15:13:38]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1440,6 +1440,21 @@
         <v>1144</v>
       </c>
     </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/15</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>1144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-16 15:12:33]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C66"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1455,6 +1455,21 @@
         <v>1144</v>
       </c>
     </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/16</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>1146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-17 15:09:23]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1470,6 +1470,21 @@
         <v>1146</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/17</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>1147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-18 15:08:58]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1485,6 +1485,21 @@
         <v>1147</v>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/18</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>1146</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-19 15:15:39]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1500,6 +1500,21 @@
         <v>1146</v>
       </c>
     </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/19</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>1149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-20 15:19:06]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1515,6 +1515,21 @@
         <v>1149</v>
       </c>
     </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/20</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>1149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-21 15:19:01]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1530,6 +1530,21 @@
         <v>1149</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/21</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>1153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-22 15:18:24]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1545,6 +1545,21 @@
         <v>1153</v>
       </c>
     </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/22</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>1155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-23 15:14:22]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1560,6 +1560,21 @@
         <v>1155</v>
       </c>
     </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/23</t>
+        </is>
+      </c>
+      <c r="B74" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>1156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-24 15:09:22]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1575,6 +1575,21 @@
         <v>1156</v>
       </c>
     </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/24</t>
+        </is>
+      </c>
+      <c r="B75" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>1156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-25 15:09:32]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1590,6 +1590,21 @@
         <v>1156</v>
       </c>
     </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/25</t>
+        </is>
+      </c>
+      <c r="B76" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>1159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-26 15:17:41]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1605,6 +1605,21 @@
         <v>1159</v>
       </c>
     </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/26</t>
+        </is>
+      </c>
+      <c r="B77" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>1159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-27 15:19:40]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1620,6 +1620,21 @@
         <v>1159</v>
       </c>
     </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/27</t>
+        </is>
+      </c>
+      <c r="B78" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>1160</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-28 15:20:11]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1635,6 +1635,21 @@
         <v>1160</v>
       </c>
     </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/28</t>
+        </is>
+      </c>
+      <c r="B79" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>1161</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-29 15:23:34]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1650,6 +1650,21 @@
         <v>1161</v>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/29</t>
+        </is>
+      </c>
+      <c r="B80" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>1164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-30 15:22:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1665,6 +1665,21 @@
         <v>1164</v>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/30</t>
+        </is>
+      </c>
+      <c r="B81" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>1167</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-01-31 15:11:21]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1680,6 +1680,21 @@
         <v>1167</v>
       </c>
     </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>2026/01/31</t>
+        </is>
+      </c>
+      <c r="B82" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>1168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-01 15:13:16]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1695,6 +1695,21 @@
         <v>1168</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/01</t>
+        </is>
+      </c>
+      <c r="B83" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>1168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-02 15:29:07]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1710,6 +1710,21 @@
         <v>1168</v>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/02</t>
+        </is>
+      </c>
+      <c r="B84" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>1170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-03 15:37:48]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1725,6 +1725,21 @@
         <v>1170</v>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/03</t>
+        </is>
+      </c>
+      <c r="B85" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>1170</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-04 15:30:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1740,6 +1740,21 @@
         <v>1170</v>
       </c>
     </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/04</t>
+        </is>
+      </c>
+      <c r="B86" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>1171</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-05 15:30:38]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1755,6 +1755,21 @@
         <v>1171</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/05</t>
+        </is>
+      </c>
+      <c r="B87" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>1174</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-06 15:29:05]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1770,6 +1770,21 @@
         <v>1174</v>
       </c>
     </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/06</t>
+        </is>
+      </c>
+      <c r="B88" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>1175</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-07 15:13:58]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1785,6 +1785,21 @@
         <v>1175</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/07</t>
+        </is>
+      </c>
+      <c r="B89" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>1181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-08 15:14:18]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1800,6 +1800,21 @@
         <v>1181</v>
       </c>
     </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/08</t>
+        </is>
+      </c>
+      <c r="B90" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>1184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-09 15:42:32]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1815,6 +1815,21 @@
         <v>1184</v>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/09</t>
+        </is>
+      </c>
+      <c r="B91" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>1185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-10 15:54:24]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1830,6 +1830,21 @@
         <v>1185</v>
       </c>
     </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/10</t>
+        </is>
+      </c>
+      <c r="B92" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>1183</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-11 15:46:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C92"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1845,6 +1845,21 @@
         <v>1183</v>
       </c>
     </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/11</t>
+        </is>
+      </c>
+      <c r="B93" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>1189</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-12 15:39:19]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1860,6 +1860,21 @@
         <v>1189</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/12</t>
+        </is>
+      </c>
+      <c r="B94" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>1190</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-13 15:30:30]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C94"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1875,6 +1875,21 @@
         <v>1190</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/13</t>
+        </is>
+      </c>
+      <c r="B95" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>1200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-14 15:14:09]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1890,6 +1890,21 @@
         <v>1200</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/14</t>
+        </is>
+      </c>
+      <c r="B96" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>1202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-15 15:14:32]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1905,6 +1905,21 @@
         <v>1202</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/15</t>
+        </is>
+      </c>
+      <c r="B97" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>1208</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-16 15:30:09]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1920,6 +1920,21 @@
         <v>1208</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/16</t>
+        </is>
+      </c>
+      <c r="B98" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>1210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-17 15:39:18]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1935,6 +1935,21 @@
         <v>1210</v>
       </c>
     </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/17</t>
+        </is>
+      </c>
+      <c r="B99" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>1210</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-18 15:38:53]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1950,6 +1950,21 @@
         <v>1210</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/18</t>
+        </is>
+      </c>
+      <c r="B100" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>1212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-19 15:35:20]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1965,6 +1965,21 @@
         <v>1212</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/19</t>
+        </is>
+      </c>
+      <c r="B101" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>1212</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-20 15:28:11]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1980,6 +1980,21 @@
         <v>1212</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/20</t>
+        </is>
+      </c>
+      <c r="B102" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>1213</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-21 15:13:15]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1995,6 +1995,21 @@
         <v>1213</v>
       </c>
     </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/21</t>
+        </is>
+      </c>
+      <c r="B103" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>1215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-22 15:13:34]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2010,6 +2010,21 @@
         <v>1215</v>
       </c>
     </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/22</t>
+        </is>
+      </c>
+      <c r="B104" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>1221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-23 15:35:35]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2025,6 +2025,21 @@
         <v>1221</v>
       </c>
     </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/23</t>
+        </is>
+      </c>
+      <c r="B105" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>1225</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-24 15:43:25]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2040,6 +2040,21 @@
         <v>1225</v>
       </c>
     </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/24</t>
+        </is>
+      </c>
+      <c r="B106" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>1228</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update mods data [2026-02-25 15:47:32]
</commit_message>
<xml_diff>
--- a/excel/逃离鸭科夫-Mods数量统计.xlsx
+++ b/excel/逃离鸭科夫-Mods数量统计.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2055,6 +2055,21 @@
         <v>1228</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>2026/02/25</t>
+        </is>
+      </c>
+      <c r="B107" s="1" t="inlineStr">
+        <is>
+          <t>逃离鸭科夫</t>
+        </is>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>1230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>